<commit_message>
chore: upload file model
</commit_message>
<xml_diff>
--- a/public/uploads/church_members_model.xlsx
+++ b/public/uploads/church_members_model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeldigbeu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aroligroup2009-my.sharepoint.com/personal/joeldigbeu_aroligroup2009_onmicrosoft_com/Documents/Documents/FREELANCE/APP VHONNEUR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D516C28E-85E3-498A-AC33-46C38C29D86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_E68F4205BEB07C5CF060021590509F77A0299751" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FEB32BC-497C-4551-A120-ADAC66E426D1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,18 +59,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,16 +85,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,12 +432,13 @@
   <dimension ref="A1:J915"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="21.75" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="22.875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="23.25" customWidth="1"/>
@@ -464,10 +454,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -490,12 +480,6 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
     </row>
     <row r="908" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J908" t="s">
@@ -540,7 +524,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C1:J1 J908:J915 A1" numberStoredAsText="1"/>
+    <ignoredError sqref="D1:J1 J908:J915" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>